<commit_message>
P7012: Change term `SD-BY` to `SD-BASE`
The core form of the agreements has been changed from `SD-BY` to
`SD-BASE` following a similar change in the P7012 document. The
rationale for this is that `BY` was adopted from `CC-BY` and `BASE`
instead represents that the suffixes to it are additions to the base
terms. This closes #378.

Co-authored-by: Iain Henderson <iain@jlinc.com>
Co-authored-by: Beatriz Esteves <beatriz.gc.esteves@gmail.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/p7012.xlsx
+++ b/code/vocab_csv/p7012.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="719">
   <si>
     <t>Term</t>
   </si>
@@ -596,7 +596,7 @@
     <t>PrivacyTerm types</t>
   </si>
   <si>
-    <t>SD-BY</t>
+    <t>SD-BASE</t>
   </si>
   <si>
     <t>Term that requires Service Delivery, and prohibits Analytics, Tracking, or Profiling by 2nd and 3rd Party, and prohibits sharing any data with 3rd Party</t>
@@ -608,25 +608,25 @@
     <t>p7012:ServiceDeliveryRequired</t>
   </si>
   <si>
-    <t>SD-BY-DP</t>
-  </si>
-  <si>
-    <t>SD BY-DP</t>
+    <t>SD-BASE-DP</t>
+  </si>
+  <si>
+    <t>SD BASE-DP</t>
   </si>
   <si>
     <t>Term that requires Service Delivery, with an obligation for Data Portability, and prohibits Analytics, Tracking, or Profiling by 2nd and 3rd Party, and prohibits sharing any data with 3rd Party</t>
   </si>
   <si>
-    <t>p7012:SD-BY</t>
+    <t>p7012:SD-BASE</t>
   </si>
   <si>
     <t>p7012:ServiceDeliveryRequired,p7012:PortabilityRequired</t>
   </si>
   <si>
-    <t>SD-BY-A</t>
-  </si>
-  <si>
-    <t>SD BY-A</t>
+    <t>SD-BASE-A</t>
+  </si>
+  <si>
+    <t>SD BASE-A</t>
   </si>
   <si>
     <t>Term that requires Service Delivery and permits Analytics, and prohibits Analytics by 3rd Party, prohibits Tracking, or Profiling by 2nd and 3rd Party, and prohibits sharing any data with 3rd Party</t>
@@ -638,28 +638,28 @@
     <t>p7012:Analytics3PDisallowed,p7012:TrackingDisallowed,p7012:ProfilingDisallowed,p7012:DataSharingDisallowed</t>
   </si>
   <si>
-    <t>SD-BY-A-DP</t>
-  </si>
-  <si>
-    <t>SD BY-A-DP</t>
+    <t>SD-BASE-A-DP</t>
+  </si>
+  <si>
+    <t>SD BASE-A-DP</t>
   </si>
   <si>
     <t>Term that requires Service Delivery and permits Analytics, with an obligation for Data Portability, and prohibits Analytics by 3rd Party, prohibits Tracking or Profiling by 2nd and 3rd Party, and prohibits sharing any data with 3rd Party</t>
   </si>
   <si>
-    <t>p7012:SD-BY-A,p7012:SD-BY-DP</t>
-  </si>
-  <si>
-    <t>SD-BY-AT</t>
-  </si>
-  <si>
-    <t>SD BY-AT</t>
+    <t>p7012:SD-BASE-A,p7012:SD-BASE-DP</t>
+  </si>
+  <si>
+    <t>SD-BASE-AT</t>
+  </si>
+  <si>
+    <t>SD BASE-AT</t>
   </si>
   <si>
     <t>Term that requires Service Delivery, and permits Analytics and Tracking by the 2nd Party, and prohibits Analytics, or Tracking by 3rd Party, prohibits Profiling by 2nd and 3rd Party, and prohibits sharing any data with 3rd Party</t>
   </si>
   <si>
-    <t>p7012:SD-BY-A</t>
+    <t>p7012:SD-BASE-A</t>
   </si>
   <si>
     <t>p7012:Analytics2PAllowed,p7012:Tracking2PAllowed</t>
@@ -668,28 +668,28 @@
     <t>p7012:Analytics3PDisallowed,p7012:Tracking3PDisallowed,p7012:ProfilingDisallowed,p7012:DataSharingDisallowed</t>
   </si>
   <si>
-    <t>SD-BY-AT-DP</t>
-  </si>
-  <si>
-    <t>SD BY-AT-DP</t>
+    <t>SD-BASE-AT-DP</t>
+  </si>
+  <si>
+    <t>SD BASE-AT-DP</t>
   </si>
   <si>
     <t>Term that requires Service Delivery, and permits Analytics and Tracking by the 2nd Party, with an obligation for Data Portability, and prohibits Analytics or Tracking by 3rd Party, prohibits Profiling by 2nd and 3rd Party, and prohibits sharing any data with 3rd Party</t>
   </si>
   <si>
-    <t>p7012:SD-BY-AT,p7012:SD-BY-DP</t>
-  </si>
-  <si>
-    <t>SD-BY-ATP</t>
-  </si>
-  <si>
-    <t>SD BY-ATP</t>
+    <t>p7012:SD-BASE-AT,p7012:SD-BASE-DP</t>
+  </si>
+  <si>
+    <t>SD-BASE-ATP</t>
+  </si>
+  <si>
+    <t>SD BASE-ATP</t>
   </si>
   <si>
     <t>Term that requires Service Delivery, and permits Analytics, Tracking, or Profiling by the 2nd party, and prohibits Analytics, Tracking, or Profiling by 3rd Party, and prohibits sharing any data with 3rd Party</t>
   </si>
   <si>
-    <t>p7012:SD-BY-AT</t>
+    <t>p7012:SD-BASE-AT</t>
   </si>
   <si>
     <t>p7012:Analytics2PAllowed,p7012:Tracking2PAllowed
@@ -699,28 +699,28 @@
     <t>p7012:Analytics3PDisallowed,p7012:Tracking3PDisallowed,p7012:Profiling3PDisallowed,p7012:DataSharingDisallowed</t>
   </si>
   <si>
-    <t>SD-BY-ATP-DP</t>
-  </si>
-  <si>
-    <t>SD BY-ATP-DP</t>
+    <t>SD-BASE-ATP-DP</t>
+  </si>
+  <si>
+    <t>SD BASE-ATP-DP</t>
   </si>
   <si>
     <t>Term that requires Service Delivery, and permits Analytics, Tracking, or Profiling by the 2nd Party, with an obligation for Data Portability, and prohibits Analytics, Tracking, or Profiling by 3rd Party, and prohibits sharing any data with 3rd Party</t>
   </si>
   <si>
-    <t>p7012:SD-BY-ATP,p7012:SD-BY-DP</t>
-  </si>
-  <si>
-    <t>SD-BY-ATP-S3P</t>
-  </si>
-  <si>
-    <t>SD BY-ATP-S3P</t>
+    <t>p7012:SD-BASE-ATP,p7012:SD-BASE-DP</t>
+  </si>
+  <si>
+    <t>SD-BASE-ATP-S3P</t>
+  </si>
+  <si>
+    <t>SD BASE-ATP-S3P</t>
   </si>
   <si>
     <t>Term that requires Service Delivery, and permits Analytics, Tracking, or Profiling by the 2nd Party, and permits sharing data that has been fully anonymised with 3rd Party, and prohibits Analytics, Tracking, or Profiling by 3rd Party, and prohibits sharing on non-anonymised data with 3rd Party</t>
   </si>
   <si>
-    <t>p7012:SD-BY-ATP</t>
+    <t>p7012:SD-BASE-ATP</t>
   </si>
   <si>
     <t>p7012:Analytics2PAllowed,p7012:Tracking2PAllowed
@@ -730,16 +730,16 @@
     <t>p7012:Analytics3PDisallowed,p7012:Tracking3PDisallowed,p7012:Profiling3PDisallowed,p7012:SharingDataNonAnonymised3PDisallowed</t>
   </si>
   <si>
-    <t>SD-BY-ATP-S3P-DP</t>
-  </si>
-  <si>
-    <t>SD BY-ATP-S3P-DP</t>
+    <t>SD-BASE-ATP-S3P-DP</t>
+  </si>
+  <si>
+    <t>SD BASE-ATP-S3P-DP</t>
   </si>
   <si>
     <t>Term that requires Service Delivery, and permits Analytics, Tracking, or Profiling by the 2nd Party, and permits sharing data that has been fully anonymised with 3rd Party, with an obligation for Data Portability, and prohibits Analytics, Tracking, Profiling by 3rd Party, and prohibits sharing on non-anonymised data with 3rd Party</t>
   </si>
   <si>
-    <t>p7012:SD-BY-ATP-S3P,p7012:SD-BY-DP</t>
+    <t>p7012:SD-BASE-ATP-S3P,p7012:SD-BASE-DP</t>
   </si>
   <si>
     <t>Personal Data Contribution</t>
@@ -1801,15 +1801,15 @@
     <t>Any Service</t>
   </si>
   <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>○</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>✓</t>
-  </si>
-  <si>
     <t>These agreements have the individual 'provide' or 'donate' data for a specific purpose/goal</t>
   </si>
   <si>
@@ -1825,13 +1825,13 @@
     <t>Legend</t>
   </si>
   <si>
-    <t>Permitted (MAY BE optionally done)</t>
-  </si>
-  <si>
-    <t>Prohibited (MUST NOT be done)</t>
-  </si>
-  <si>
-    <t>Obligation (MUST be done)</t>
+    <t>Obligation / Necessary (MUST be done)</t>
+  </si>
+  <si>
+    <t>Prohibition (MUST NOT be done)</t>
+  </si>
+  <si>
+    <t>Permission / Optional (MAY BE done)</t>
   </si>
   <si>
     <t>AgreementNegotiationStatus</t>
@@ -2445,7 +2445,7 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <font/>
       <fill>
@@ -2472,6 +2472,16 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFC9DAF8"/>
           <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
       <border/>
@@ -24363,7 +24373,7 @@
         <v>593</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="4">
@@ -24389,7 +24399,7 @@
         <v>593</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="5">
@@ -24403,7 +24413,7 @@
         <v>592</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>593</v>
@@ -24415,7 +24425,7 @@
         <v>593</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="6">
@@ -24429,7 +24439,7 @@
         <v>592</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>593</v>
@@ -24441,7 +24451,7 @@
         <v>593</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="7">
@@ -24455,10 +24465,10 @@
         <v>592</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>593</v>
@@ -24467,7 +24477,7 @@
         <v>593</v>
       </c>
       <c r="H7" s="37" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="8">
@@ -24481,10 +24491,10 @@
         <v>592</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>593</v>
@@ -24493,7 +24503,7 @@
         <v>593</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="9">
@@ -24507,19 +24517,19 @@
         <v>592</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>593</v>
       </c>
       <c r="H9" s="37" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="10">
@@ -24533,19 +24543,19 @@
         <v>592</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>593</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="11">
@@ -24559,19 +24569,19 @@
         <v>592</v>
       </c>
       <c r="D11" s="14" t="s">
+        <v>592</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>592</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>592</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>592</v>
+      </c>
+      <c r="H11" s="37" t="s">
         <v>594</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>594</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>594</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>594</v>
-      </c>
-      <c r="H11" s="37" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="12">
@@ -24585,19 +24595,19 @@
         <v>592</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="13">
@@ -24620,7 +24630,7 @@
         <v>596</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>593</v>
@@ -24635,7 +24645,7 @@
         <v>593</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="15">
@@ -24646,7 +24656,7 @@
         <v>597</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>593</v>
@@ -24661,7 +24671,7 @@
         <v>593</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="16">
@@ -24672,7 +24682,7 @@
         <v>598</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D16" s="41" t="s">
         <v>593</v>
@@ -24687,7 +24697,7 @@
         <v>593</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="17">
@@ -24700,12 +24710,9 @@
     </row>
     <row r="19">
       <c r="A19" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>600</v>
-      </c>
-      <c r="C19" s="14" t="s">
         <v>600</v>
       </c>
     </row>
@@ -24716,18 +24723,12 @@
       <c r="B20" s="14" t="s">
         <v>601</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>601</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="25" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>602</v>
-      </c>
-      <c r="C21" s="14" t="s">
         <v>602</v>
       </c>
     </row>
@@ -27689,6 +27690,11 @@
   <conditionalFormatting sqref="B3:H12 B14:H51">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"○"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(J6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <drawing r:id="rId1"/>

</xml_diff>